<commit_message>
Validate array type normalRange
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-vitals-validate-normal-range-in-validation-criteria.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-vitals-validate-normal-range-in-validation-criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC3E8E0-8520-854C-A678-FC1686F6DA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4E526-C1B9-9E47-B95D-A32DB137153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="5840" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="4640" windowWidth="33640" windowHeight="22040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>Temperature (°C)</t>
   </si>
   <si>
-    <t>{"min": 32, "max": 44, "normalRange": {"min": 35.5, "max": 37.5}}</t>
-  </si>
-  <si>
     <t>pde-PatientVitalsSPO2</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>{"min": 1, "max": 70}</t>
+  </si>
+  <si>
+    <t>{"min": 32, "max": 44, "normalRange": [{"min": 120, "max": 185, "ageUnit": "months", "ageMin": 0, "ageMax": 3}]}</t>
   </si>
 </sst>
 </file>
@@ -1837,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1887,7 +1887,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>30</v>
@@ -1991,7 +1991,7 @@
         <v>53</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2011,10 +2011,10 @@
         <v>56</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2034,10 +2034,10 @@
         <v>59</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2099,10 +2099,10 @@
         <v>69</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2121,60 +2121,60 @@
       <c r="E11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>73</v>
+      <c r="L11" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="M13" s="2"/>
     </row>
@@ -2183,85 +2183,85 @@
     </row>
     <row r="15" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="M18" s="2"/>
     </row>

</xml_diff>